<commit_message>
Subir version beta v1
</commit_message>
<xml_diff>
--- a/Proyecto/Documentacion/Casos de prueba.xlsx
+++ b/Proyecto/Documentacion/Casos de prueba.xlsx
@@ -5,6 +5,10 @@
   <sheets>
     <sheet state="visible" name="El alumno contesta encuesta" sheetId="1" r:id="rId3"/>
     <sheet state="visible" name="El administrador registra alumn" sheetId="2" r:id="rId4"/>
+    <sheet state="visible" name="El administrador registra grupo" sheetId="3" r:id="rId5"/>
+    <sheet state="visible" name="El administrador contacta alumn" sheetId="4" r:id="rId6"/>
+    <sheet state="visible" name="Publicar encuesta" sheetId="5" r:id="rId7"/>
+    <sheet state="visible" name="La directora consulta reportes" sheetId="6" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="120">
   <si>
     <t>Nombre escenario</t>
   </si>
@@ -33,6 +37,9 @@
   </si>
   <si>
     <t>2. El alumno ya contestó la encuesta</t>
+  </si>
+  <si>
+    <t>Cancelar operacion</t>
   </si>
   <si>
     <t xml:space="preserve">A2 </t>
@@ -45,6 +52,9 @@
     <t>A3</t>
   </si>
   <si>
+    <t>El archivo no esta normalizado</t>
+  </si>
+  <si>
     <t>4. Registro encuesta exitoso</t>
   </si>
   <si>
@@ -63,6 +73,9 @@
     <t>Token</t>
   </si>
   <si>
+    <t>Registro alumnos exitoso</t>
+  </si>
+  <si>
     <t>Anterior</t>
   </si>
   <si>
@@ -81,12 +94,24 @@
     <t>V</t>
   </si>
   <si>
+    <t>Archivo</t>
+  </si>
+  <si>
+    <t>Normaliziado</t>
+  </si>
+  <si>
     <t>F</t>
   </si>
   <si>
+    <t>Confirmar</t>
+  </si>
+  <si>
     <t>Mensaje Gracias por contestar la encuesta 'Alumno.nombre'</t>
   </si>
   <si>
+    <t>No completo campos obligatorios</t>
+  </si>
+  <si>
     <t>RC 2</t>
   </si>
   <si>
@@ -129,12 +154,42 @@
     <t>TI token</t>
   </si>
   <si>
+    <t>Mensaje : se ha cancelado la operacoion</t>
+  </si>
+  <si>
+    <t>Mensaje de error: El archivo que subiste no cumple los lineamientos establecidos</t>
+  </si>
+  <si>
+    <t>El nombre del grupo esta duplicado</t>
+  </si>
+  <si>
+    <t>El archivo no es válido</t>
+  </si>
+  <si>
+    <t>Mensaje de error: No subiste ningun archivo</t>
+  </si>
+  <si>
+    <t>Registro grupos  exitoso</t>
+  </si>
+  <si>
+    <t>Mensaje de error: Los alumnos han sido registrados</t>
+  </si>
+  <si>
+    <t>A Archivo</t>
+  </si>
+  <si>
     <t>T token real</t>
   </si>
   <si>
+    <t>C Confirmado</t>
+  </si>
+  <si>
     <t>HA hora actual</t>
   </si>
   <si>
+    <t>N normalizado</t>
+  </si>
+  <si>
     <t>H- hora mínima</t>
   </si>
   <si>
@@ -147,9 +202,30 @@
     <t>C campos obligatorios contestados</t>
   </si>
   <si>
+    <t>Mensaje de error: te falta completar los campos obligatorios</t>
+  </si>
+  <si>
     <t>A ya habia contestado con anterioridad la encuesta</t>
   </si>
   <si>
+    <t>Mensaje de error: El nombre del grupo esta duplicado, favor de cambiarlo</t>
+  </si>
+  <si>
+    <t>Mensaje de error: El grupo ha sido registrado</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Ca Campos</t>
+  </si>
+  <si>
     <t>HA</t>
   </si>
   <si>
@@ -165,13 +241,10 @@
     <t>T</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>CO</t>
   </si>
   <si>
-    <t>C</t>
+    <t>Ca</t>
   </si>
   <si>
     <t>10/04/18
@@ -188,13 +261,136 @@
   <si>
     <t>01/06/18
 00:00</t>
+  </si>
+  <si>
+    <t>RF: haber hecho una consulta</t>
+  </si>
+  <si>
+    <t>Fecha anterior a la actual elegida</t>
+  </si>
+  <si>
+    <t>Cancela contactar</t>
+  </si>
+  <si>
+    <t>Seleccionar reporte historico</t>
+  </si>
+  <si>
+    <t>Integridad del archivo subido (oferta laboral)</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>Los filtros no retornan alumnos</t>
+  </si>
+  <si>
+    <t>Contacto de alumnos exitoso</t>
+  </si>
+  <si>
+    <t>Cancelar la operación</t>
+  </si>
+  <si>
+    <t>Los filtros retornan alumnos</t>
+  </si>
+  <si>
+    <t>Más reportes</t>
+  </si>
+  <si>
+    <t>Regreso lista alumnos</t>
+  </si>
+  <si>
+    <t>Confirmado</t>
+  </si>
+  <si>
+    <t>Fecha de inicio posterior a fecha de fin</t>
+  </si>
+  <si>
+    <t>Mensjae de error: no llego a los filtros</t>
+  </si>
+  <si>
+    <t>Mensaje de error: El archivo seleccionado aun no se ha subido</t>
+  </si>
+  <si>
+    <t>Target no seleccionado</t>
+  </si>
+  <si>
+    <t>Mensaje de error: no se encontro ningun alumno acorde a los filtros seleccionados</t>
+  </si>
+  <si>
+    <t>Mensaje: se ha enviado la oferta / contactado a los alumnos seleccionados</t>
+  </si>
+  <si>
+    <t>Publicación exitosa</t>
+  </si>
+  <si>
+    <t>Mensaje de error: se cancelo la consulta</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>Mensaje:  lista de alumnos por filtro</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>FechaInicio</t>
+  </si>
+  <si>
+    <t>FechaFin</t>
+  </si>
+  <si>
+    <t>FechaActual</t>
+  </si>
+  <si>
+    <t>Mensjae de error: no puedes publicar a un dia anterior del actual</t>
+  </si>
+  <si>
+    <t>Mensaje de error: la fecha fin no puede ser antes de la fehca inicio</t>
+  </si>
+  <si>
+    <t>Mensaje de error: Necesitas seleccionar al menos un grupo/target para publicarles la encuesta</t>
+  </si>
+  <si>
+    <t>Mensaje:  se ha publicado la encuesta</t>
+  </si>
+  <si>
+    <t>T Target</t>
+  </si>
+  <si>
+    <t>FF FechaFin</t>
+  </si>
+  <si>
+    <t>FI FechaInicio</t>
+  </si>
+  <si>
+    <t>FA FechaActual</t>
+  </si>
+  <si>
+    <t>FI</t>
+  </si>
+  <si>
+    <t>FF</t>
+  </si>
+  <si>
+    <t>FA</t>
+  </si>
+  <si>
+    <t>Alumnos de 6BPV</t>
+  </si>
+  <si>
+    <t>NULL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -205,6 +401,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -234,7 +431,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -244,7 +441,25 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -258,6 +473,22 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
@@ -311,265 +542,265 @@
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2"/>
     </row>
     <row r="24">
-      <c r="A24" s="3"/>
+      <c r="A24" s="4"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="F26" s="1">
         <v>5.64161351E8</v>
@@ -578,7 +809,7 @@
         <v>5.64161351E8</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="I26" s="1">
         <v>10.0</v>
@@ -587,24 +818,24 @@
         <v>10.0</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="F27" s="1">
         <v>5.64161351E8</v>
@@ -613,7 +844,7 @@
         <v>5.64161351E8</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="I27" s="1">
         <v>10.0</v>
@@ -622,24 +853,24 @@
         <v>5.0</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="F28" s="1">
         <v>5.64161351E8</v>
@@ -648,33 +879,33 @@
         <v>5.64161351E8</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="F29" s="1">
         <v>65313.0</v>
@@ -683,58 +914,58 @@
         <v>5.64161351E8</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="3"/>
+      <c r="A31" s="4"/>
     </row>
     <row r="32">
-      <c r="A32" s="3"/>
+      <c r="A32" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -754,7 +985,8 @@
     <col customWidth="1" min="1" max="1" width="34.29"/>
     <col customWidth="1" min="2" max="2" width="52.86"/>
     <col customWidth="1" min="3" max="3" width="10.86"/>
-    <col customWidth="1" min="4" max="5" width="9.14"/>
+    <col customWidth="1" min="4" max="4" width="12.57"/>
+    <col customWidth="1" min="5" max="5" width="10.0"/>
     <col customWidth="1" min="6" max="6" width="11.43"/>
     <col customWidth="1" min="7" max="7" width="12.29"/>
     <col customWidth="1" min="8" max="9" width="7.29"/>
@@ -774,7 +1006,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -785,127 +1017,861 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="4"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="4"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="34.29"/>
+    <col customWidth="1" min="2" max="2" width="52.86"/>
+    <col customWidth="1" min="3" max="3" width="10.86"/>
+    <col customWidth="1" min="4" max="4" width="12.57"/>
+    <col customWidth="1" min="5" max="5" width="10.0"/>
+    <col customWidth="1" min="6" max="6" width="11.43"/>
+    <col customWidth="1" min="7" max="7" width="12.29"/>
+    <col customWidth="1" min="8" max="9" width="7.29"/>
+    <col customWidth="1" min="10" max="10" width="7.43"/>
+  </cols>
+  <sheetData>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="4"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="4"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="33.14"/>
+    <col customWidth="1" min="2" max="2" width="28.71"/>
+    <col customWidth="1" min="3" max="3" width="10.71"/>
+    <col customWidth="1" min="4" max="4" width="12.57"/>
+    <col customWidth="1" min="5" max="5" width="10.0"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>82</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>26</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>28</v>
+        <v>87</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="4"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="4"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="36.29"/>
+    <col customWidth="1" min="2" max="2" width="52.86"/>
+    <col customWidth="1" min="3" max="3" width="17.29"/>
+    <col customWidth="1" min="4" max="4" width="12.57"/>
+    <col customWidth="1" min="5" max="5" width="11.43"/>
+    <col customWidth="1" min="6" max="6" width="12.43"/>
+    <col customWidth="1" min="7" max="8" width="11.43"/>
+    <col customWidth="1" min="9" max="9" width="12.29"/>
+    <col customWidth="1" min="10" max="11" width="7.29"/>
+    <col customWidth="1" min="12" max="12" width="7.43"/>
+  </cols>
+  <sheetData>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="D9" s="6">
+        <v>43517.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>21</v>
       </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="D11" s="1" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="12">
@@ -913,22 +1879,25 @@
         <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>93</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="13">
@@ -936,285 +1905,484 @@
         <v>34</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>35</v>
+        <v>96</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="H13" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="s">
-        <v>38</v>
+      <c r="A15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>39</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>40</v>
+        <v>112</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="2" t="s">
-        <v>41</v>
+      <c r="A19" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>42</v>
+        <v>114</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>43</v>
+        <v>54</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="2" t="s">
-        <v>44</v>
+      <c r="A22" s="2"/>
+      <c r="B22" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2"/>
     </row>
     <row r="24">
-      <c r="A24" s="3"/>
+      <c r="A24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" s="1"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>13</v>
+        <v>81</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>48</v>
+        <v>118</v>
+      </c>
+      <c r="D25" s="7">
+        <v>43153.0</v>
+      </c>
+      <c r="E25" s="8">
+        <v>43524.0</v>
+      </c>
+      <c r="F25" s="8">
+        <v>43517.0</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>18</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="I25" s="1"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>20</v>
+        <v>93</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>53</v>
+        <v>118</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F26" s="1">
-        <v>5.64161351E8</v>
-      </c>
-      <c r="G26" s="1">
-        <v>5.64161351E8</v>
+        <v>27</v>
+      </c>
+      <c r="F26" s="8">
+        <v>43517.0</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I26" s="1">
-        <v>10.0</v>
-      </c>
-      <c r="J26" s="1">
-        <v>10.0</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>23</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="I26" s="1"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>25</v>
+        <v>96</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>53</v>
+        <v>119</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F27" s="1">
-        <v>5.64161351E8</v>
-      </c>
-      <c r="G27" s="1">
-        <v>5.64161351E8</v>
+        <v>36</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I27" s="1">
-        <v>10.0</v>
-      </c>
-      <c r="J27" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>26</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="I27" s="1"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>28</v>
+        <v>99</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F28" s="1">
-        <v>5.64161351E8</v>
-      </c>
-      <c r="G28" s="1">
-        <v>5.64161351E8</v>
+        <v>118</v>
+      </c>
+      <c r="D28" s="7">
+        <v>43518.0</v>
+      </c>
+      <c r="E28" s="8">
+        <v>43524.0</v>
+      </c>
+      <c r="F28" s="8">
+        <v>43517.0</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="H28" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D29" s="7">
+        <v>43518.0</v>
+      </c>
+      <c r="E29" s="7">
+        <v>43518.0</v>
+      </c>
+      <c r="F29" s="8">
+        <v>43517.0</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="4"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="4"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="36.29"/>
+    <col customWidth="1" min="2" max="2" width="52.86"/>
+    <col customWidth="1" min="3" max="3" width="10.86"/>
+    <col customWidth="1" min="4" max="4" width="12.57"/>
+    <col customWidth="1" min="5" max="5" width="10.0"/>
+    <col customWidth="1" min="6" max="7" width="11.43"/>
+    <col customWidth="1" min="8" max="8" width="12.29"/>
+    <col customWidth="1" min="9" max="10" width="7.29"/>
+    <col customWidth="1" min="11" max="11" width="7.43"/>
+  </cols>
+  <sheetData>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="s">
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F29" s="1">
-        <v>65313.0</v>
-      </c>
-      <c r="G29" s="1">
-        <v>5.64161351E8</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="s">
+      <c r="B11" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="3"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="3"/>
+      <c r="B12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="4"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Add v1.1 del sistema + base de datos + docs
</commit_message>
<xml_diff>
--- a/Proyecto/Documentacion/Casos de prueba.xlsx
+++ b/Proyecto/Documentacion/Casos de prueba.xlsx
@@ -36,13 +36,19 @@
     <t>A1</t>
   </si>
   <si>
+    <t>Cancelar operacion</t>
+  </si>
+  <si>
     <t>2. El alumno ya contestó la encuesta</t>
   </si>
   <si>
-    <t>Cancelar operacion</t>
-  </si>
-  <si>
     <t xml:space="preserve">A2 </t>
+  </si>
+  <si>
+    <t>No completo campos obligatorios</t>
+  </si>
+  <si>
+    <t>El archivo no esta normalizado</t>
   </si>
   <si>
     <t xml:space="preserve">3. No contestó todos los campos
@@ -52,28 +58,43 @@
     <t>A3</t>
   </si>
   <si>
-    <t>El archivo no esta normalizado</t>
+    <t>Registro alumnos exitoso</t>
   </si>
   <si>
     <t>4. Registro encuesta exitoso</t>
   </si>
   <si>
+    <t>El nombre del grupo esta duplicado</t>
+  </si>
+  <si>
     <t>A4</t>
   </si>
   <si>
     <t>ID</t>
   </si>
   <si>
+    <t>Registro grupos  exitoso</t>
+  </si>
+  <si>
     <t>Escenario</t>
   </si>
   <si>
+    <t>Archivo</t>
+  </si>
+  <si>
+    <t>Normaliziado</t>
+  </si>
+  <si>
     <t>Fecha</t>
   </si>
   <si>
+    <t>Confirmar</t>
+  </si>
+  <si>
     <t>Token</t>
   </si>
   <si>
-    <t>Registro alumnos exitoso</t>
+    <t>Resultado esperado</t>
   </si>
   <si>
     <t>Anterior</t>
@@ -82,60 +103,63 @@
     <t>Campos</t>
   </si>
   <si>
-    <t>Resultado esperado</t>
-  </si>
-  <si>
     <t>RC 1</t>
   </si>
   <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Mensaje : se ha cancelado la operacoion</t>
+  </si>
+  <si>
     <t>Registro encuesta exitoso</t>
   </si>
   <si>
-    <t>V</t>
-  </si>
-  <si>
-    <t>Archivo</t>
-  </si>
-  <si>
-    <t>Normaliziado</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>Confirmar</t>
+    <t>RC 2</t>
   </si>
   <si>
     <t>Mensaje Gracias por contestar la encuesta 'Alumno.nombre'</t>
   </si>
   <si>
-    <t>No completo campos obligatorios</t>
-  </si>
-  <si>
-    <t>RC 2</t>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Mensaje de error: El archivo que subiste no cumple los lineamientos establecidos</t>
+  </si>
+  <si>
+    <t>RC 3</t>
+  </si>
+  <si>
+    <t>El archivo no es válido</t>
   </si>
   <si>
     <t>No contesto todos los campos necesarios de la encuesta</t>
   </si>
   <si>
+    <t>Mensaje de error: No subiste ningun archivo</t>
+  </si>
+  <si>
+    <t>RC 4</t>
+  </si>
+  <si>
     <t>Mensaje de error: Por favor, completa los campos obligatorios faltantes</t>
   </si>
   <si>
-    <t>RC 3</t>
+    <t>Mensaje de error: Los alumnos han sido registrados</t>
+  </si>
+  <si>
+    <t>A Archivo</t>
   </si>
   <si>
     <t>El alumno ya contestó la encuesta</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>Mensaje de error: Lo sentimos, ya has contestado esta encuesta</t>
   </si>
   <si>
-    <t>RC 4</t>
-  </si>
-  <si>
     <t>Token no es válido</t>
   </si>
   <si>
@@ -154,76 +178,55 @@
     <t>TI token</t>
   </si>
   <si>
-    <t>Mensaje : se ha cancelado la operacoion</t>
-  </si>
-  <si>
-    <t>Mensaje de error: El archivo que subiste no cumple los lineamientos establecidos</t>
-  </si>
-  <si>
-    <t>El nombre del grupo esta duplicado</t>
-  </si>
-  <si>
-    <t>El archivo no es válido</t>
-  </si>
-  <si>
-    <t>Mensaje de error: No subiste ningun archivo</t>
-  </si>
-  <si>
-    <t>Registro grupos  exitoso</t>
-  </si>
-  <si>
-    <t>Mensaje de error: Los alumnos han sido registrados</t>
-  </si>
-  <si>
-    <t>A Archivo</t>
+    <t>Mensaje de error: te falta completar los campos obligatorios</t>
+  </si>
+  <si>
+    <t>Mensaje de error: El nombre del grupo esta duplicado, favor de cambiarlo</t>
+  </si>
+  <si>
+    <t>C Confirmado</t>
+  </si>
+  <si>
+    <t>N normalizado</t>
   </si>
   <si>
     <t>T token real</t>
   </si>
   <si>
-    <t>C Confirmado</t>
-  </si>
-  <si>
     <t>HA hora actual</t>
   </si>
   <si>
-    <t>N normalizado</t>
+    <t>Mensaje de error: El grupo ha sido registrado</t>
   </si>
   <si>
     <t>H- hora mínima</t>
   </si>
   <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
     <t>H+ hora máxima</t>
   </si>
   <si>
+    <t>Ca Campos</t>
+  </si>
+  <si>
     <t xml:space="preserve">CO total campos obligatorios </t>
   </si>
   <si>
     <t>C campos obligatorios contestados</t>
   </si>
   <si>
-    <t>Mensaje de error: te falta completar los campos obligatorios</t>
-  </si>
-  <si>
     <t>A ya habia contestado con anterioridad la encuesta</t>
   </si>
   <si>
-    <t>Mensaje de error: El nombre del grupo esta duplicado, favor de cambiarlo</t>
-  </si>
-  <si>
-    <t>Mensaje de error: El grupo ha sido registrado</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Ca Campos</t>
+    <t>Ca</t>
   </si>
   <si>
     <t>HA</t>
@@ -242,9 +245,6 @@
   </si>
   <si>
     <t>CO</t>
-  </si>
-  <si>
-    <t>Ca</t>
   </si>
   <si>
     <t>10/04/18
@@ -266,31 +266,40 @@
     <t>RF: haber hecho una consulta</t>
   </si>
   <si>
+    <t>Seleccionar reporte historico</t>
+  </si>
+  <si>
     <t>Fecha anterior a la actual elegida</t>
   </si>
   <si>
+    <t>Los filtros no retornan alumnos</t>
+  </si>
+  <si>
     <t>Cancela contactar</t>
   </si>
   <si>
-    <t>Seleccionar reporte historico</t>
+    <t>Cancelar la operación</t>
   </si>
   <si>
     <t>Integridad del archivo subido (oferta laboral)</t>
   </si>
   <si>
+    <t>Fecha de inicio posterior a fecha de fin</t>
+  </si>
+  <si>
     <t>A2</t>
   </si>
   <si>
-    <t>Los filtros no retornan alumnos</t>
+    <t>Los filtros retornan alumnos</t>
+  </si>
+  <si>
+    <t>Target no seleccionado</t>
   </si>
   <si>
     <t>Contacto de alumnos exitoso</t>
   </si>
   <si>
-    <t>Cancelar la operación</t>
-  </si>
-  <si>
-    <t>Los filtros retornan alumnos</t>
+    <t>Publicación exitosa</t>
   </si>
   <si>
     <t>Más reportes</t>
@@ -302,7 +311,7 @@
     <t>Confirmado</t>
   </si>
   <si>
-    <t>Fecha de inicio posterior a fecha de fin</t>
+    <t>A5</t>
   </si>
   <si>
     <t>Mensjae de error: no llego a los filtros</t>
@@ -311,52 +320,43 @@
     <t>Mensaje de error: El archivo seleccionado aun no se ha subido</t>
   </si>
   <si>
-    <t>Target no seleccionado</t>
-  </si>
-  <si>
     <t>Mensaje de error: no se encontro ningun alumno acorde a los filtros seleccionados</t>
   </si>
   <si>
     <t>Mensaje: se ha enviado la oferta / contactado a los alumnos seleccionados</t>
   </si>
   <si>
-    <t>Publicación exitosa</t>
-  </si>
-  <si>
     <t>Mensaje de error: se cancelo la consulta</t>
   </si>
   <si>
-    <t>A5</t>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>FechaInicio</t>
+  </si>
+  <si>
+    <t>FechaFin</t>
+  </si>
+  <si>
+    <t>FechaActual</t>
+  </si>
+  <si>
+    <t>Mensjae de error: no puedes publicar a un dia anterior del actual</t>
+  </si>
+  <si>
+    <t>Mensaje de error: la fecha fin no puede ser antes de la fehca inicio</t>
+  </si>
+  <si>
+    <t>Mensaje de error: Necesitas seleccionar al menos un grupo/target para publicarles la encuesta</t>
+  </si>
+  <si>
+    <t>Mensaje:  se ha publicado la encuesta</t>
+  </si>
+  <si>
+    <t>T Target</t>
   </si>
   <si>
     <t>Mensaje:  lista de alumnos por filtro</t>
-  </si>
-  <si>
-    <t>Target</t>
-  </si>
-  <si>
-    <t>FechaInicio</t>
-  </si>
-  <si>
-    <t>FechaFin</t>
-  </si>
-  <si>
-    <t>FechaActual</t>
-  </si>
-  <si>
-    <t>Mensjae de error: no puedes publicar a un dia anterior del actual</t>
-  </si>
-  <si>
-    <t>Mensaje de error: la fecha fin no puede ser antes de la fehca inicio</t>
-  </si>
-  <si>
-    <t>Mensaje de error: Necesitas seleccionar al menos un grupo/target para publicarles la encuesta</t>
-  </si>
-  <si>
-    <t>Mensaje:  se ha publicado la encuesta</t>
-  </si>
-  <si>
-    <t>T Target</t>
   </si>
   <si>
     <t>FF FechaFin</t>
@@ -445,10 +445,10 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -536,7 +536,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -547,202 +547,202 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23">
@@ -753,45 +753,45 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>76</v>
@@ -809,7 +809,7 @@
         <v>5.64161351E8</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="I26" s="1">
         <v>10.0</v>
@@ -818,15 +818,15 @@
         <v>10.0</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>76</v>
@@ -844,7 +844,7 @@
         <v>5.64161351E8</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="I27" s="1">
         <v>10.0</v>
@@ -853,15 +853,15 @@
         <v>5.0</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>76</v>
@@ -879,24 +879,24 @@
         <v>5.64161351E8</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>76</v>
@@ -914,24 +914,24 @@
         <v>5.64161351E8</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>79</v>
@@ -943,22 +943,22 @@
         <v>78</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31">
@@ -1006,7 +1006,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -1017,7 +1017,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -1028,123 +1028,123 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16">
@@ -1157,106 +1157,106 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G18" s="1"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="G19" s="1"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="G20" s="1"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="G21" s="1"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G22" s="1"/>
     </row>
@@ -1305,7 +1305,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -1316,7 +1316,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -1327,139 +1327,139 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18">
@@ -1467,106 +1467,106 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G19" s="1"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="G20" s="1"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G21" s="1"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G22" s="1"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G23" s="1"/>
     </row>
@@ -1616,7 +1616,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -1627,92 +1627,92 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13">
@@ -1764,7 +1764,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -1775,7 +1775,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -1786,201 +1786,201 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9">
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>43517.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="G10" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18">
@@ -1988,7 +1988,7 @@
         <v>112</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19">
@@ -2009,7 +2009,7 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>114</v>
@@ -2018,7 +2018,7 @@
     <row r="22">
       <c r="A22" s="2"/>
       <c r="B22" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23">
@@ -2026,13 +2026,13 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>115</v>
@@ -2044,19 +2044,19 @@
         <v>117</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="I24" s="1"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>118</v>
@@ -2071,73 +2071,73 @@
         <v>43517.0</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I25" s="1"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>118</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F26" s="8">
         <v>43517.0</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I26" s="1"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>119</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="I27" s="1"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>118</v>
@@ -2152,19 +2152,19 @@
         <v>43517.0</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I28" s="1"/>
     </row>
     <row r="29">
-      <c r="A29" s="5" t="s">
-        <v>41</v>
+      <c r="A29" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>118</v>
@@ -2179,10 +2179,10 @@
         <v>43517.0</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35">
@@ -2230,7 +2230,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -2241,7 +2241,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -2252,13 +2252,13 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
@@ -2269,107 +2269,107 @@
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="5" t="s">
-        <v>38</v>
+      <c r="A13" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>89</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16">

</xml_diff>